<commit_message>
Correción de error multiples: matriz de más en el json y variables con letras separadas y en Mayúsculas
</commit_message>
<xml_diff>
--- a/Hojas de Cálculo/elementos.xlsx
+++ b/Hojas de Cálculo/elementos.xlsx
@@ -22,19 +22,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="108">
   <si>
-    <t xml:space="preserve">A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nombre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Simbolo Químico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Valencias</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Repeticion</t>
+    <t xml:space="preserve">a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nombre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">repeticion</t>
   </si>
   <si>
     <t xml:space="preserve">Hidrógeno</t>
@@ -358,6 +358,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -379,6 +380,7 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -396,6 +398,7 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -544,10 +547,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="260" zoomScaleNormal="260" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.04"/>

</xml_diff>

<commit_message>
He modificado la hoja de cálculo porque estab mal. También he hecho una función que me crea una matriz con una casilla por cada repetición de cada elemento.
</commit_message>
<xml_diff>
--- a/Hojas de Cálculo/elementos.xlsx
+++ b/Hojas de Cálculo/elementos.xlsx
@@ -55,12 +55,90 @@
     <t xml:space="preserve">Al</t>
   </si>
   <si>
+    <t xml:space="preserve">Arsénico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,-3,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Au</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Boro</t>
   </si>
   <si>
     <t xml:space="preserve">B </t>
   </si>
   <si>
+    <t xml:space="preserve">Bario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Berilio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Be</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bromo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Br</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,3,5,-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carbono</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,4,-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calcio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cadmio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cloro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,3,5,7-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cobalto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Co</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cromo</t>
   </si>
   <si>
@@ -70,6 +148,12 @@
     <t xml:space="preserve">2,3,6</t>
   </si>
   <si>
+    <t xml:space="preserve">Cesio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cs</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cobre</t>
   </si>
   <si>
@@ -79,13 +163,22 @@
     <t xml:space="preserve">1,2</t>
   </si>
   <si>
+    <t xml:space="preserve">Flúor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hierro</t>
   </si>
   <si>
     <t xml:space="preserve">Fe</t>
   </si>
   <si>
-    <t xml:space="preserve">2,3</t>
+    <t xml:space="preserve">Francio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fr</t>
   </si>
   <si>
     <t xml:space="preserve">Galio</t>
@@ -94,12 +187,45 @@
     <t xml:space="preserve">Ga</t>
   </si>
   <si>
+    <t xml:space="preserve">Hidrógeno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,-1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mercurio</t>
   </si>
   <si>
     <t xml:space="preserve">Hg</t>
   </si>
   <si>
+    <t xml:space="preserve">Yodo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potasio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Litio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Li</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magnesio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Manganeso</t>
   </si>
   <si>
@@ -109,48 +235,108 @@
     <t xml:space="preserve">2,3,4,6,7</t>
   </si>
   <si>
+    <t xml:space="preserve">Nitrógeno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sodio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Na</t>
+  </si>
+  <si>
     <t xml:space="preserve">Níquel</t>
   </si>
   <si>
     <t xml:space="preserve">Ni</t>
   </si>
   <si>
+    <t xml:space="preserve">Oxigeno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1,-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fósforo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plomo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,4</t>
+  </si>
+  <si>
     <t xml:space="preserve">Paladio</t>
   </si>
   <si>
     <t xml:space="preserve">Pd</t>
   </si>
   <si>
-    <t xml:space="preserve">2,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Au</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cadmio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cobalto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Co</t>
-  </si>
-  <si>
     <t xml:space="preserve">Platino</t>
   </si>
   <si>
     <t xml:space="preserve">Pt</t>
   </si>
   <si>
+    <t xml:space="preserve">Radio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rubidio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Azufre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,4,6,-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Selenio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silicio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Si</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estaño</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estroncio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sr</t>
+  </si>
+  <si>
     <t xml:space="preserve">Titanio</t>
   </si>
   <si>
@@ -160,196 +346,10 @@
     <t xml:space="preserve">2,3,4</t>
   </si>
   <si>
-    <t xml:space="preserve">Plomo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pb</t>
-  </si>
-  <si>
     <t xml:space="preserve">Cinc</t>
   </si>
   <si>
     <t xml:space="preserve">Zn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calcio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flúor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yodo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,3,5,7-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Litio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Li</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fósforo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,-3,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Azufre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,4,6,-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Selenio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Se</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Silicio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Si</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4,-4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estroncio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Berilio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Be</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bromo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Br</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,3,5,-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Carbono</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,4,-4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cloro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Magnesio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nitrógeno</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sodio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Na</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Radio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rubidio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Francio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hidrógeno</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oxigeno</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1,-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arsénico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cesio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Potasio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estaño</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sn</t>
   </si>
 </sst>
 </file>
@@ -547,20 +547,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFF10D0C"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="260" zoomScaleNormal="260" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="F42" activeCellId="0" sqref="F42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="E46" activeCellId="0" sqref="E46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.04"/>
@@ -601,7 +601,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="4" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>2</v>
@@ -621,7 +621,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>2</v>
@@ -629,7 +629,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>10</v>
@@ -637,31 +637,31 @@
       <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="3" t="n">
-        <v>3</v>
+      <c r="D4" s="0" t="s">
+        <v>12</v>
       </c>
       <c r="E4" s="4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>24</v>
+        <v>79</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="0" t="s">
         <v>14</v>
       </c>
+      <c r="D5" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="E5" s="4" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>2</v>
@@ -669,19 +669,19 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="D6" s="3" t="n">
+        <v>3</v>
+      </c>
       <c r="E6" s="4" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>2</v>
@@ -689,7 +689,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>18</v>
@@ -697,59 +697,59 @@
       <c r="C7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>20</v>
+      <c r="D7" s="3" t="n">
+        <v>2</v>
       </c>
       <c r="E7" s="4" t="n">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="D8" s="3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E8" s="4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>80</v>
+        <v>36</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="E9" s="4" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>25</v>
@@ -761,15 +761,15 @@
         <v>27</v>
       </c>
       <c r="E10" s="4" t="n">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>28</v>
@@ -777,19 +777,19 @@
       <c r="C11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>20</v>
+      <c r="D11" s="3" t="n">
+        <v>2</v>
       </c>
       <c r="E11" s="4" t="n">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>30</v>
@@ -797,11 +797,11 @@
       <c r="C12" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="0" t="s">
-        <v>32</v>
+      <c r="D12" s="3" t="n">
+        <v>2</v>
       </c>
       <c r="E12" s="4" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>2</v>
@@ -809,39 +809,39 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>79</v>
+        <v>17</v>
       </c>
       <c r="B13" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="E13" s="4" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="B14" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="3" t="n">
-        <v>2</v>
-      </c>
       <c r="E14" s="4" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>2</v>
@@ -849,7 +849,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>38</v>
@@ -857,11 +857,11 @@
       <c r="C15" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>20</v>
+      <c r="D15" s="0" t="s">
+        <v>40</v>
       </c>
       <c r="E15" s="4" t="n">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>2</v>
@@ -869,39 +869,39 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>32</v>
+        <v>42</v>
+      </c>
+      <c r="D16" s="3" t="n">
+        <v>1</v>
       </c>
       <c r="E16" s="4" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="F16" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" s="0" t="s">
         <v>44</v>
       </c>
+      <c r="D17" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="E17" s="4" t="n">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>2</v>
@@ -909,39 +909,39 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
-        <v>82</v>
+        <v>9</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>32</v>
+        <v>47</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>-1</v>
       </c>
       <c r="E18" s="4" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F18" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D19" s="3" t="n">
-        <v>2</v>
+        <v>49</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="E19" s="4" t="n">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>2</v>
@@ -949,19 +949,19 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D20" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20" s="4" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F20" s="0" t="n">
         <v>5</v>
@@ -969,79 +969,79 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D21" s="0" t="n">
-        <v>-1</v>
+        <v>53</v>
+      </c>
+      <c r="D21" s="3" t="n">
+        <v>3</v>
       </c>
       <c r="E21" s="4" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="F21" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E22" s="4" t="n">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="F22" s="0" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
-        <v>3</v>
+        <v>80</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D23" s="3" t="n">
-        <v>1</v>
+        <v>58</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="E23" s="4" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F23" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="E24" s="4" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F24" s="0" t="n">
         <v>5</v>
@@ -1049,7 +1049,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>61</v>
@@ -1057,11 +1057,11 @@
       <c r="C25" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D25" s="0" t="s">
-        <v>63</v>
+      <c r="D25" s="3" t="n">
+        <v>1</v>
       </c>
       <c r="E25" s="4" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F25" s="0" t="n">
         <v>5</v>
@@ -1069,19 +1069,19 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="B26" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>63</v>
+      <c r="D26" s="3" t="n">
+        <v>1</v>
       </c>
       <c r="E26" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F26" s="0" t="n">
         <v>5</v>
@@ -1089,19 +1089,19 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B27" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>68</v>
+      <c r="D27" s="3" t="n">
+        <v>2</v>
       </c>
       <c r="E27" s="4" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F27" s="0" t="n">
         <v>5</v>
@@ -1109,39 +1109,39 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="B28" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D28" s="3" t="n">
-        <v>2</v>
-      </c>
       <c r="E28" s="4" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F28" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="4" t="n">
         <v>4</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D29" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="E29" s="4" t="n">
-        <v>10</v>
       </c>
       <c r="F29" s="0" t="n">
         <v>5</v>
@@ -1149,19 +1149,19 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="B30" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D30" s="0" t="s">
-        <v>75</v>
+      <c r="D30" s="3" t="n">
+        <v>1</v>
       </c>
       <c r="E30" s="4" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="F30" s="0" t="n">
         <v>5</v>
@@ -1169,59 +1169,59 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>78</v>
+        <v>75</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="E31" s="4" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F31" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="E32" s="4" t="n">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="F32" s="0" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D33" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B33" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D33" s="3" t="n">
-        <v>2</v>
-      </c>
       <c r="E33" s="4" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F33" s="0" t="n">
         <v>5</v>
@@ -1229,79 +1229,79 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
-        <v>7</v>
+        <v>82</v>
       </c>
       <c r="B34" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D34" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>60</v>
-      </c>
       <c r="E34" s="4" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F34" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="B35" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D35" s="3" t="n">
-        <v>1</v>
+      <c r="D35" s="0" t="s">
+        <v>83</v>
       </c>
       <c r="E35" s="4" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F35" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B36" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D36" s="3" t="n">
-        <v>2</v>
+      <c r="D36" s="0" t="s">
+        <v>83</v>
       </c>
       <c r="E36" s="4" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F36" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
-        <v>37</v>
+        <v>88</v>
       </c>
       <c r="B37" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>90</v>
-      </c>
       <c r="D37" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E37" s="4" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F37" s="0" t="n">
         <v>5</v>
@@ -1309,19 +1309,19 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="B38" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>92</v>
-      </c>
       <c r="D38" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E38" s="4" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F38" s="0" t="n">
         <v>5</v>
@@ -1329,19 +1329,19 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
-        <v>87</v>
+        <v>16</v>
       </c>
       <c r="B39" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="D39" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="D39" s="3" t="n">
-        <v>1</v>
-      </c>
       <c r="E39" s="4" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F39" s="0" t="n">
         <v>5</v>
@@ -1349,7 +1349,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="B40" s="0" t="s">
         <v>95</v>
@@ -1358,70 +1358,70 @@
         <v>96</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E40" s="4" t="n">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="F40" s="0" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B41" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="D41" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="D41" s="0" t="s">
-        <v>100</v>
-      </c>
       <c r="E41" s="4" t="n">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="F41" s="0" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="B42" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>102</v>
-      </c>
       <c r="D42" s="0" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="E42" s="4" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F42" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="B43" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>104</v>
-      </c>
       <c r="D43" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E43" s="4" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F43" s="0" t="n">
         <v>5</v>
@@ -1429,27 +1429,27 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B44" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="D44" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="D44" s="3" t="n">
-        <v>1</v>
-      </c>
       <c r="E44" s="4" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F44" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="B45" s="0" t="s">
         <v>107</v>
@@ -1457,11 +1457,11 @@
       <c r="C45" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D45" s="0" t="s">
-        <v>32</v>
+      <c r="D45" s="3" t="n">
+        <v>2</v>
       </c>
       <c r="E45" s="4" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F45" s="0" t="n">
         <v>2</v>

</xml_diff>

<commit_message>
Utilización de un srcipt en R para pasar de *.xlsx a JSON y añadir a la hoja de cálculo el grupo de cada elemento para identificar los ácidos
</commit_message>
<xml_diff>
--- a/Hojas de Cálculo/elementos.xlsx
+++ b/Hojas de Cálculo/elementos.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="110">
   <si>
     <t xml:space="preserve">a</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t xml:space="preserve">puntos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grupo</t>
   </si>
   <si>
     <t xml:space="preserve">Plata</t>
@@ -552,15 +555,15 @@
     <tabColor rgb="FFF10D0C"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E46" activeCellId="0" sqref="E46"/>
+      <selection pane="bottomLeft" activeCell="G45" activeCellId="0" sqref="G45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.04"/>
@@ -586,16 +589,19 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>47</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="3" t="n">
         <v>1</v>
@@ -605,6 +611,9 @@
       </c>
       <c r="F2" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -612,10 +621,10 @@
         <v>13</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" s="3" t="n">
         <v>3</v>
@@ -625,6 +634,9 @@
       </c>
       <c r="F3" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -632,19 +644,22 @@
         <v>33</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E4" s="4" t="n">
         <v>1</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -652,19 +667,22 @@
         <v>79</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E5" s="4" t="n">
         <v>1</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -672,10 +690,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D6" s="3" t="n">
         <v>3</v>
@@ -685,6 +703,9 @@
       </c>
       <c r="F6" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -692,10 +713,10 @@
         <v>56</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D7" s="3" t="n">
         <v>2</v>
@@ -705,6 +726,9 @@
       </c>
       <c r="F7" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -712,10 +736,10 @@
         <v>4</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D8" s="3" t="n">
         <v>2</v>
@@ -725,6 +749,9 @@
       </c>
       <c r="F8" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -732,19 +759,22 @@
         <v>36</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E9" s="4" t="n">
         <v>5</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -752,19 +782,22 @@
         <v>6</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E10" s="4" t="n">
         <v>3</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -772,10 +805,10 @@
         <v>20</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D11" s="3" t="n">
         <v>2</v>
@@ -785,6 +818,9 @@
       </c>
       <c r="F11" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -792,10 +828,10 @@
         <v>48</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D12" s="3" t="n">
         <v>2</v>
@@ -805,6 +841,9 @@
       </c>
       <c r="F12" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -812,19 +851,22 @@
         <v>17</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E13" s="4" t="n">
         <v>5</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -832,19 +874,22 @@
         <v>27</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E14" s="4" t="n">
         <v>1</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -852,19 +897,22 @@
         <v>24</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E15" s="4" t="n">
         <v>2</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -872,10 +920,10 @@
         <v>55</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D16" s="3" t="n">
         <v>1</v>
@@ -885,6 +933,9 @@
       </c>
       <c r="F16" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -892,19 +943,22 @@
         <v>29</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E17" s="4" t="n">
         <v>2</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -912,10 +966,10 @@
         <v>9</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>-1</v>
@@ -925,6 +979,9 @@
       </c>
       <c r="F18" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -932,19 +989,22 @@
         <v>26</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E19" s="4" t="n">
         <v>2</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -952,10 +1012,10 @@
         <v>87</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D20" s="3" t="n">
         <v>1</v>
@@ -965,6 +1025,9 @@
       </c>
       <c r="F20" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -972,10 +1035,10 @@
         <v>31</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D21" s="3" t="n">
         <v>3</v>
@@ -986,25 +1049,31 @@
       <c r="F21" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="G21" s="0" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E22" s="4" t="n">
         <v>28</v>
       </c>
       <c r="F22" s="0" t="n">
         <v>10</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1012,19 +1081,22 @@
         <v>80</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E23" s="4" t="n">
         <v>1</v>
       </c>
       <c r="F23" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1032,19 +1104,22 @@
         <v>53</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E24" s="4" t="n">
         <v>3</v>
       </c>
       <c r="F24" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1052,10 +1127,10 @@
         <v>19</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D25" s="3" t="n">
         <v>1</v>
@@ -1065,6 +1140,9 @@
       </c>
       <c r="F25" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1072,10 +1150,10 @@
         <v>3</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D26" s="3" t="n">
         <v>1</v>
@@ -1085,6 +1163,9 @@
       </c>
       <c r="F26" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1092,10 +1173,10 @@
         <v>12</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D27" s="3" t="n">
         <v>2</v>
@@ -1105,6 +1186,9 @@
       </c>
       <c r="F27" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1112,19 +1196,22 @@
         <v>25</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E28" s="4" t="n">
         <v>2</v>
       </c>
       <c r="F28" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="G28" s="0" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1132,19 +1219,22 @@
         <v>7</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E29" s="4" t="n">
         <v>4</v>
       </c>
       <c r="F29" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="G29" s="0" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1152,10 +1242,10 @@
         <v>11</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D30" s="3" t="n">
         <v>1</v>
@@ -1165,6 +1255,9 @@
       </c>
       <c r="F30" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="G30" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1172,19 +1265,22 @@
         <v>28</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E31" s="4" t="n">
         <v>1</v>
       </c>
       <c r="F31" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="G31" s="0" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1192,19 +1288,22 @@
         <v>8</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E32" s="4" t="n">
         <v>37</v>
       </c>
       <c r="F32" s="0" t="n">
         <v>10</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1212,19 +1311,22 @@
         <v>15</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E33" s="4" t="n">
         <v>3</v>
       </c>
       <c r="F33" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="G33" s="0" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1232,19 +1334,22 @@
         <v>82</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E34" s="4" t="n">
         <v>1</v>
       </c>
       <c r="F34" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="G34" s="0" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1252,19 +1357,22 @@
         <v>46</v>
       </c>
       <c r="B35" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D35" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D35" s="0" t="s">
-        <v>83</v>
-      </c>
       <c r="E35" s="4" t="n">
         <v>1</v>
       </c>
       <c r="F35" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="G35" s="0" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1272,19 +1380,22 @@
         <v>78</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E36" s="4" t="n">
         <v>1</v>
       </c>
       <c r="F36" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="G36" s="0" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1292,10 +1403,10 @@
         <v>88</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D37" s="3" t="n">
         <v>2</v>
@@ -1305,6 +1416,9 @@
       </c>
       <c r="F37" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="G37" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1312,10 +1426,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D38" s="3" t="n">
         <v>1</v>
@@ -1325,6 +1439,9 @@
       </c>
       <c r="F38" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="G38" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1332,19 +1449,22 @@
         <v>16</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E39" s="4" t="n">
         <v>5</v>
       </c>
       <c r="F39" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="G39" s="0" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1352,19 +1472,22 @@
         <v>34</v>
       </c>
       <c r="B40" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D40" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D40" s="0" t="s">
-        <v>94</v>
-      </c>
       <c r="E40" s="4" t="n">
         <v>1</v>
       </c>
       <c r="F40" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="G40" s="0" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1372,19 +1495,22 @@
         <v>14</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E41" s="4" t="n">
         <v>1</v>
       </c>
       <c r="F41" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="G41" s="0" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1392,19 +1518,22 @@
         <v>50</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E42" s="4" t="n">
         <v>1</v>
       </c>
       <c r="F42" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="G42" s="0" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1412,10 +1541,10 @@
         <v>38</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D43" s="3" t="n">
         <v>2</v>
@@ -1425,6 +1554,9 @@
       </c>
       <c r="F43" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="G43" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1432,19 +1564,22 @@
         <v>22</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E44" s="4" t="n">
         <v>1</v>
       </c>
       <c r="F44" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="G44" s="0" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1452,10 +1587,10 @@
         <v>30</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D45" s="3" t="n">
         <v>2</v>
@@ -1465,6 +1600,9 @@
       </c>
       <c r="F45" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="G45" s="0" t="n">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
He sustituido la a por la z
</commit_message>
<xml_diff>
--- a/Hojas de Cálculo/elementos.xlsx
+++ b/Hojas de Cálculo/elementos.xlsx
@@ -25,7 +25,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="110">
   <si>
-    <t xml:space="preserve">a</t>
+    <t xml:space="preserve">z</t>
   </si>
   <si>
     <t xml:space="preserve">nombre</t>
@@ -550,7 +550,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <tabColor rgb="FFF10D0C"/>
     <pageSetUpPr fitToPage="false"/>
@@ -558,16 +558,19 @@
   <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G45" activeCellId="0" sqref="G45"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
He acabado de editar los componentes
</commit_message>
<xml_diff>
--- a/Hojas de Cálculo/elementos.xlsx
+++ b/Hojas de Cálculo/elementos.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="111">
   <si>
     <t xml:space="preserve">z</t>
   </si>
@@ -64,7 +64,7 @@
     <t xml:space="preserve">As</t>
   </si>
   <si>
-    <t xml:space="preserve">3,-3,5</t>
+    <t xml:space="preserve">-3,3,5</t>
   </si>
   <si>
     <t xml:space="preserve">Oro</t>
@@ -100,7 +100,7 @@
     <t xml:space="preserve">Br</t>
   </si>
   <si>
-    <t xml:space="preserve">1,3,5,-1</t>
+    <t xml:space="preserve">-1,1,3,5</t>
   </si>
   <si>
     <t xml:space="preserve">Carbono</t>
@@ -109,7 +109,7 @@
     <t xml:space="preserve">C</t>
   </si>
   <si>
-    <t xml:space="preserve">2,4,-4</t>
+    <t xml:space="preserve">-4,2,4</t>
   </si>
   <si>
     <t xml:space="preserve">Calcio</t>
@@ -130,7 +130,7 @@
     <t xml:space="preserve">Cl</t>
   </si>
   <si>
-    <t xml:space="preserve">1,3,5,7-1</t>
+    <t xml:space="preserve">-1,1,3,5,7</t>
   </si>
   <si>
     <t xml:space="preserve">Cobalto</t>
@@ -196,7 +196,7 @@
     <t xml:space="preserve">H</t>
   </si>
   <si>
-    <t xml:space="preserve">1,-1</t>
+    <t xml:space="preserve">-1,1</t>
   </si>
   <si>
     <t xml:space="preserve">Mercurio</t>
@@ -310,7 +310,7 @@
     <t xml:space="preserve">S</t>
   </si>
   <si>
-    <t xml:space="preserve">2,4,6,-2</t>
+    <t xml:space="preserve">-2,2,4,6</t>
   </si>
   <si>
     <t xml:space="preserve">Selenio</t>
@@ -319,13 +319,16 @@
     <t xml:space="preserve">Se</t>
   </si>
   <si>
+    <t xml:space="preserve">-2,2,4,7</t>
+  </si>
+  <si>
     <t xml:space="preserve">Silicio</t>
   </si>
   <si>
     <t xml:space="preserve">Si</t>
   </si>
   <si>
-    <t xml:space="preserve">4,-4</t>
+    <t xml:space="preserve">-4,4</t>
   </si>
   <si>
     <t xml:space="preserve">Estaño</t>
@@ -550,7 +553,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFF10D0C"/>
     <pageSetUpPr fitToPage="false"/>
@@ -558,19 +561,16 @@
   <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="D47" activeCellId="0" sqref="D47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1481,7 +1481,7 @@
         <v>97</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="E40" s="4" t="n">
         <v>1</v>
@@ -1498,13 +1498,13 @@
         <v>14</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E41" s="4" t="n">
         <v>1</v>
@@ -1521,10 +1521,10 @@
         <v>50</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D42" s="0" t="s">
         <v>84</v>
@@ -1544,10 +1544,10 @@
         <v>38</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D43" s="3" t="n">
         <v>2</v>
@@ -1567,13 +1567,13 @@
         <v>22</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E44" s="4" t="n">
         <v>1</v>
@@ -1590,10 +1590,10 @@
         <v>30</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D45" s="3" t="n">
         <v>2</v>

</xml_diff>

<commit_message>
He añadido formato a las tarjetas
</commit_message>
<xml_diff>
--- a/Hojas de Cálculo/elementos.xlsx
+++ b/Hojas de Cálculo/elementos.xlsx
@@ -11,8 +11,9 @@
     <sheet name="Total" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Total!$B$1:$H$45</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Total!$A$1:$F$45</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Total!$A$1:$F$45</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Total!$A$1:$H$45</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Total!$B$1:$H$45</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="120">
   <si>
     <t xml:space="preserve">z</t>
   </si>
@@ -47,7 +48,7 @@
     <t xml:space="preserve">grupo</t>
   </si>
   <si>
-    <t xml:space="preserve">Tipo</t>
+    <t xml:space="preserve">tipo</t>
   </si>
   <si>
     <t xml:space="preserve">Cesio</t>
@@ -56,7 +57,7 @@
     <t xml:space="preserve">Cs</t>
   </si>
   <si>
-    <t xml:space="preserve">Grupo _1</t>
+    <t xml:space="preserve">Grupo1</t>
   </si>
   <si>
     <t xml:space="preserve">Francio</t>
@@ -104,7 +105,7 @@
     <t xml:space="preserve">Ba</t>
   </si>
   <si>
-    <t xml:space="preserve">Grupo_2</t>
+    <t xml:space="preserve">Grupo2</t>
   </si>
   <si>
     <t xml:space="preserve">Berilio</t>
@@ -137,9 +138,6 @@
     <t xml:space="preserve">Ca</t>
   </si>
   <si>
-    <t xml:space="preserve">Grupo _2</t>
-  </si>
-  <si>
     <t xml:space="preserve">Titanio</t>
   </si>
   <si>
@@ -254,7 +252,7 @@
     <t xml:space="preserve">Al</t>
   </si>
   <si>
-    <t xml:space="preserve">Grupo_13</t>
+    <t xml:space="preserve">Grupo13</t>
   </si>
   <si>
     <t xml:space="preserve">Boro</t>
@@ -278,7 +276,7 @@
     <t xml:space="preserve">-4,2,4</t>
   </si>
   <si>
-    <t xml:space="preserve">Grupo_14</t>
+    <t xml:space="preserve">Grupo14</t>
   </si>
   <si>
     <t xml:space="preserve">Plomo</t>
@@ -311,7 +309,7 @@
     <t xml:space="preserve">-3,3,5</t>
   </si>
   <si>
-    <t xml:space="preserve">Grupo_15</t>
+    <t xml:space="preserve">Grupo15</t>
   </si>
   <si>
     <t xml:space="preserve">Nitrógeno</t>
@@ -335,7 +333,7 @@
     <t xml:space="preserve">-1,-2</t>
   </si>
   <si>
-    <t xml:space="preserve">Grupo_16</t>
+    <t xml:space="preserve">Grupo16</t>
   </si>
   <si>
     <t xml:space="preserve">Azufre</t>
@@ -365,7 +363,7 @@
     <t xml:space="preserve">-1,1,3,5</t>
   </si>
   <si>
-    <t xml:space="preserve">Grupo_17</t>
+    <t xml:space="preserve">Grupo17</t>
   </si>
   <si>
     <t xml:space="preserve">Cloro</t>
@@ -595,15 +593,16 @@
   </sheetPr>
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="H45" activeCellId="0" sqref="H45"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.93"/>
   </cols>
@@ -636,7 +635,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>8</v>
@@ -662,7 +661,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>13</v>
+        <v>87</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>11</v>
@@ -688,7 +687,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>13</v>
@@ -714,7 +713,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>79</v>
+        <v>19</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>16</v>
@@ -740,7 +739,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>18</v>
@@ -766,7 +765,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>20</v>
@@ -792,7 +791,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>22</v>
@@ -818,7 +817,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>24</v>
@@ -844,7 +843,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>27</v>
@@ -870,7 +869,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>29</v>
@@ -896,7 +895,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>48</v>
+        <v>88</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>31</v>
@@ -922,7 +921,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>33</v>
@@ -948,7 +947,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>35</v>
@@ -969,21 +968,21 @@
         <v>2</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B15" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="D15" s="0" t="s">
         <v>39</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>40</v>
       </c>
       <c r="E15" s="5" t="n">
         <v>1</v>
@@ -995,21 +994,21 @@
         <v>4</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="B16" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="0" t="s">
         <v>43</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>44</v>
       </c>
       <c r="E16" s="5" t="n">
         <v>2</v>
@@ -1021,21 +1020,21 @@
         <v>6</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B17" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="D17" s="0" t="s">
         <v>46</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>47</v>
       </c>
       <c r="E17" s="5" t="n">
         <v>2</v>
@@ -1047,21 +1046,21 @@
         <v>7</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="B18" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="D18" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>50</v>
       </c>
       <c r="E18" s="5" t="n">
         <v>2</v>
@@ -1073,21 +1072,21 @@
         <v>8</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B19" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="D19" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E19" s="5" t="n">
         <v>1</v>
@@ -1099,21 +1098,21 @@
         <v>9</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
-        <v>87</v>
+        <v>28</v>
       </c>
       <c r="B20" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>54</v>
-      </c>
       <c r="D20" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E20" s="5" t="n">
         <v>1</v>
@@ -1125,21 +1124,21 @@
         <v>10</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="B21" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="D21" s="0" t="s">
         <v>56</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>57</v>
       </c>
       <c r="E21" s="5" t="n">
         <v>1</v>
@@ -1151,21 +1150,21 @@
         <v>10</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
-        <v>1</v>
+        <v>78</v>
       </c>
       <c r="B22" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="D22" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E22" s="5" t="n">
         <v>1</v>
@@ -1177,18 +1176,18 @@
         <v>10</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
-        <v>80</v>
+        <v>47</v>
       </c>
       <c r="B23" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="D23" s="4" t="n">
         <v>1</v>
@@ -1203,21 +1202,21 @@
         <v>11</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
-        <v>53</v>
+        <v>79</v>
       </c>
       <c r="B24" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="D24" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>64</v>
       </c>
       <c r="E24" s="5" t="n">
         <v>1</v>
@@ -1229,21 +1228,21 @@
         <v>11</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B25" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="D25" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>67</v>
       </c>
       <c r="E25" s="5" t="n">
         <v>2</v>
@@ -1255,18 +1254,18 @@
         <v>11</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="B26" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>69</v>
       </c>
       <c r="D26" s="4" t="n">
         <v>2</v>
@@ -1281,21 +1280,21 @@
         <v>12</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
-        <v>12</v>
+        <v>80</v>
       </c>
       <c r="B27" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>71</v>
-      </c>
       <c r="D27" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E27" s="5" t="n">
         <v>1</v>
@@ -1307,18 +1306,18 @@
         <v>12</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B28" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>73</v>
       </c>
       <c r="D28" s="4" t="n">
         <v>2</v>
@@ -1333,18 +1332,18 @@
         <v>12</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B29" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="D29" s="4" t="n">
         <v>3</v>
@@ -1359,18 +1358,18 @@
         <v>13</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B30" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>78</v>
       </c>
       <c r="D30" s="4" t="n">
         <v>3</v>
@@ -1385,18 +1384,18 @@
         <v>13</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B31" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>80</v>
       </c>
       <c r="D31" s="4" t="n">
         <v>3</v>
@@ -1411,21 +1410,21 @@
         <v>13</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B32" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="D32" s="0" t="s">
         <v>82</v>
-      </c>
-      <c r="D32" s="0" t="s">
-        <v>83</v>
       </c>
       <c r="E32" s="5" t="n">
         <v>3</v>
@@ -1437,21 +1436,21 @@
         <v>14</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
-        <v>15</v>
+        <v>82</v>
       </c>
       <c r="B33" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>86</v>
-      </c>
       <c r="D33" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E33" s="5" t="n">
         <v>1</v>
@@ -1462,22 +1461,22 @@
       <c r="G33" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="H33" s="2" t="s">
-        <v>84</v>
+      <c r="H33" s="0" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
-        <v>82</v>
+        <v>14</v>
       </c>
       <c r="B34" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="D34" s="0" t="s">
         <v>88</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>89</v>
       </c>
       <c r="E34" s="5" t="n">
         <v>1</v>
@@ -1488,22 +1487,22 @@
       <c r="G34" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="H34" s="2" t="s">
-        <v>84</v>
+      <c r="H34" s="0" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B35" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>91</v>
-      </c>
       <c r="D35" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E35" s="5" t="n">
         <v>1</v>
@@ -1514,22 +1513,22 @@
       <c r="G35" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="H35" s="2" t="s">
-        <v>84</v>
+      <c r="H35" s="0" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
-        <v>78</v>
+        <v>33</v>
       </c>
       <c r="B36" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="D36" s="0" t="s">
         <v>93</v>
-      </c>
-      <c r="D36" s="0" t="s">
-        <v>94</v>
       </c>
       <c r="E36" s="5" t="n">
         <v>1</v>
@@ -1541,21 +1540,21 @@
         <v>15</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
-        <v>88</v>
+        <v>7</v>
       </c>
       <c r="B37" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>97</v>
-      </c>
       <c r="D37" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E37" s="5" t="n">
         <v>4</v>
@@ -1567,21 +1566,21 @@
         <v>15</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="B38" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>99</v>
-      </c>
       <c r="D38" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E38" s="5" t="n">
         <v>3</v>
@@ -1593,21 +1592,21 @@
         <v>15</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B39" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="D39" s="0" t="s">
         <v>101</v>
-      </c>
-      <c r="D39" s="0" t="s">
-        <v>102</v>
       </c>
       <c r="E39" s="5" t="n">
         <v>37</v>
@@ -1619,21 +1618,21 @@
         <v>16</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="B40" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="D40" s="0" t="s">
         <v>105</v>
-      </c>
-      <c r="D40" s="0" t="s">
-        <v>106</v>
       </c>
       <c r="E40" s="5" t="n">
         <v>5</v>
@@ -1645,21 +1644,21 @@
         <v>16</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B41" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="D41" s="0" t="s">
         <v>108</v>
-      </c>
-      <c r="D41" s="0" t="s">
-        <v>109</v>
       </c>
       <c r="E41" s="5" t="n">
         <v>1</v>
@@ -1671,21 +1670,21 @@
         <v>16</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="B42" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="D42" s="0" t="s">
         <v>111</v>
-      </c>
-      <c r="D42" s="0" t="s">
-        <v>112</v>
       </c>
       <c r="E42" s="5" t="n">
         <v>5</v>
@@ -1697,21 +1696,21 @@
         <v>17</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="B43" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="D43" s="0" t="s">
         <v>115</v>
-      </c>
-      <c r="D43" s="0" t="s">
-        <v>116</v>
       </c>
       <c r="E43" s="5" t="n">
         <v>5</v>
@@ -1723,18 +1722,18 @@
         <v>17</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B44" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="C44" s="3" t="s">
         <v>117</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>118</v>
       </c>
       <c r="D44" s="0" t="n">
         <v>-1</v>
@@ -1749,21 +1748,21 @@
         <v>17</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="B45" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="C45" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C45" s="3" t="s">
-        <v>120</v>
-      </c>
       <c r="D45" s="0" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E45" s="5" t="n">
         <v>3</v>
@@ -1775,11 +1774,11 @@
         <v>17</v>
       </c>
       <c r="H45" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:H45"/>
+  <autoFilter ref="A1:F45"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
He creado una hoja de cálculo con los nombres de los Anfígenos y Halógenos
</commit_message>
<xml_diff>
--- a/Hojas de Cálculo/elementos.xlsx
+++ b/Hojas de Cálculo/elementos.xlsx
@@ -11,10 +11,10 @@
     <sheet name="Total" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Total!$A$1:$H$87</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Total!$A$1:$H$45</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Total!$A$1:$F$45</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Total!$B$1:$H$45</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Total!$A$1:$H$45</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Total!$A$1:$H$87</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Total!$A$1:$F$45</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Total!$B$1:$H$45</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="121">
   <si>
     <t xml:space="preserve">z</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t xml:space="preserve">-4,2,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yhh</t>
   </si>
   <si>
     <t xml:space="preserve">Grupo14</t>
@@ -587,7 +590,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <tabColor rgb="FFF10D0C"/>
     <pageSetUpPr fitToPage="false"/>
@@ -597,15 +600,17 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1:H87"/>
+      <selection pane="bottomLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.79"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -754,14 +759,14 @@
       <c r="E6" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="F6" s="0" t="n">
-        <v>5</v>
+      <c r="F6" s="0" t="s">
+        <v>23</v>
       </c>
       <c r="G6" s="0" t="n">
         <v>14</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -769,13 +774,13 @@
         <v>7</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E7" s="4" t="n">
         <v>4</v>
@@ -787,7 +792,7 @@
         <v>15</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -795,13 +800,13 @@
         <v>8</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E8" s="4" t="n">
         <v>37</v>
@@ -813,7 +818,7 @@
         <v>16</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -821,10 +826,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>-1</v>
@@ -839,7 +844,7 @@
         <v>17</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -847,10 +852,10 @@
         <v>11</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D10" s="5" t="n">
         <v>1</v>
@@ -873,10 +878,10 @@
         <v>12</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D11" s="5" t="n">
         <v>2</v>
@@ -899,10 +904,10 @@
         <v>13</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D12" s="5" t="n">
         <v>3</v>
@@ -925,13 +930,13 @@
         <v>14</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E13" s="4" t="n">
         <v>1</v>
@@ -943,7 +948,7 @@
         <v>14</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -951,13 +956,13 @@
         <v>15</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E14" s="4" t="n">
         <v>3</v>
@@ -969,7 +974,7 @@
         <v>15</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -977,13 +982,13 @@
         <v>16</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E15" s="4" t="n">
         <v>5</v>
@@ -995,7 +1000,7 @@
         <v>16</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1003,13 +1008,13 @@
         <v>17</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E16" s="4" t="n">
         <v>5</v>
@@ -1021,7 +1026,7 @@
         <v>17</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1029,10 +1034,10 @@
         <v>19</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D17" s="5" t="n">
         <v>1</v>
@@ -1055,10 +1060,10 @@
         <v>20</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D18" s="5" t="n">
         <v>2</v>
@@ -1081,13 +1086,13 @@
         <v>22</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E19" s="4" t="n">
         <v>1</v>
@@ -1099,7 +1104,7 @@
         <v>4</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1107,13 +1112,13 @@
         <v>24</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E20" s="4" t="n">
         <v>2</v>
@@ -1125,7 +1130,7 @@
         <v>6</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1133,13 +1138,13 @@
         <v>25</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E21" s="4" t="n">
         <v>2</v>
@@ -1151,7 +1156,7 @@
         <v>7</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1159,13 +1164,13 @@
         <v>26</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E22" s="4" t="n">
         <v>2</v>
@@ -1177,7 +1182,7 @@
         <v>8</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1185,13 +1190,13 @@
         <v>27</v>
       </c>
       <c r="B23" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>69</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>68</v>
       </c>
       <c r="E23" s="4" t="n">
         <v>1</v>
@@ -1203,7 +1208,7 @@
         <v>9</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1211,13 +1216,13 @@
         <v>28</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E24" s="4" t="n">
         <v>1</v>
@@ -1229,7 +1234,7 @@
         <v>10</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1237,13 +1242,13 @@
         <v>29</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E25" s="4" t="n">
         <v>2</v>
@@ -1255,7 +1260,7 @@
         <v>11</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1263,10 +1268,10 @@
         <v>30</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D26" s="5" t="n">
         <v>2</v>
@@ -1281,7 +1286,7 @@
         <v>12</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1289,10 +1294,10 @@
         <v>31</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D27" s="5" t="n">
         <v>3</v>
@@ -1315,13 +1320,13 @@
         <v>33</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E28" s="4" t="n">
         <v>1</v>
@@ -1333,7 +1338,7 @@
         <v>15</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1341,13 +1346,13 @@
         <v>34</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E29" s="4" t="n">
         <v>1</v>
@@ -1359,7 +1364,7 @@
         <v>16</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1367,13 +1372,13 @@
         <v>35</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E30" s="4" t="n">
         <v>5</v>
@@ -1385,7 +1390,7 @@
         <v>17</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1393,10 +1398,10 @@
         <v>37</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D31" s="5" t="n">
         <v>1</v>
@@ -1419,10 +1424,10 @@
         <v>38</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D32" s="5" t="n">
         <v>2</v>
@@ -1445,13 +1450,13 @@
         <v>46</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E33" s="4" t="n">
         <v>1</v>
@@ -1463,7 +1468,7 @@
         <v>10</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1471,10 +1476,10 @@
         <v>47</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D34" s="5" t="n">
         <v>1</v>
@@ -1489,7 +1494,7 @@
         <v>11</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1497,10 +1502,10 @@
         <v>48</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D35" s="5" t="n">
         <v>2</v>
@@ -1515,7 +1520,7 @@
         <v>12</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1523,13 +1528,13 @@
         <v>50</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E36" s="4" t="n">
         <v>1</v>
@@ -1541,7 +1546,7 @@
         <v>14</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1549,13 +1554,13 @@
         <v>53</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E37" s="4" t="n">
         <v>3</v>
@@ -1567,7 +1572,7 @@
         <v>17</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1575,10 +1580,10 @@
         <v>55</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D38" s="5" t="n">
         <v>1</v>
@@ -1601,10 +1606,10 @@
         <v>56</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D39" s="5" t="n">
         <v>2</v>
@@ -1627,13 +1632,13 @@
         <v>78</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E40" s="4" t="n">
         <v>1</v>
@@ -1645,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1653,13 +1658,13 @@
         <v>79</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E41" s="4" t="n">
         <v>1</v>
@@ -1671,7 +1676,7 @@
         <v>11</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1679,13 +1684,13 @@
         <v>80</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E42" s="4" t="n">
         <v>1</v>
@@ -1697,7 +1702,7 @@
         <v>12</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1705,13 +1710,13 @@
         <v>82</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E43" s="4" t="n">
         <v>1</v>
@@ -1723,7 +1728,7 @@
         <v>14</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1731,10 +1736,10 @@
         <v>87</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D44" s="5" t="n">
         <v>1</v>
@@ -1757,10 +1762,10 @@
         <v>88</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D45" s="5" t="n">
         <v>2</v>
@@ -1779,7 +1784,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H87"/>
+  <autoFilter ref="A1:H45"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>